<commit_message>
* update bulkupload validation * update test cases
</commit_message>
<xml_diff>
--- a/docs/2010-10-11_Final Project Folder/TestCase1_30.xlsx
+++ b/docs/2010-10-11_Final Project Folder/TestCase1_30.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="422" uniqueCount="303">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="422" uniqueCount="304">
   <si>
     <t>CSSE3004/CSSE7024 Test Case</t>
     <phoneticPr fontId="0" type="noConversion"/>
@@ -942,10 +942,6 @@
     <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
-    <t>F: need to validate missing fields</t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
     <t>F: need to validate sample data  when updating</t>
     <phoneticPr fontId="6" type="noConversion"/>
   </si>
@@ -971,6 +967,14 @@
   </si>
   <si>
     <t>F: need to display confirm message</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>P</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>P</t>
     <phoneticPr fontId="6" type="noConversion"/>
   </si>
 </sst>
@@ -1501,8 +1505,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I112"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
-      <selection activeCell="E84" sqref="E84"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -1789,7 +1793,7 @@
         <v>171</v>
       </c>
       <c r="E16" s="18" t="s">
-        <v>295</v>
+        <v>302</v>
       </c>
     </row>
     <row r="17" spans="1:9" s="5" customFormat="1" ht="38.25">
@@ -1807,7 +1811,7 @@
         <v>171</v>
       </c>
       <c r="E17" s="18" t="s">
-        <v>295</v>
+        <v>303</v>
       </c>
       <c r="F17"/>
       <c r="G17"/>
@@ -1869,7 +1873,7 @@
         <v>166</v>
       </c>
       <c r="E20" s="18" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="21" spans="1:9" s="5" customFormat="1" ht="38.25">
@@ -1887,7 +1891,7 @@
         <v>166</v>
       </c>
       <c r="E21" s="18" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="F21"/>
       <c r="G21"/>
@@ -2411,7 +2415,7 @@
         <v>239</v>
       </c>
       <c r="E47" s="19" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="F47"/>
       <c r="G47"/>
@@ -3096,10 +3100,10 @@
         <v>82</v>
       </c>
       <c r="B85" s="12" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C85" s="12" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="D85" s="12" t="s">
         <v>9</v>
@@ -3138,10 +3142,10 @@
         <v>18</v>
       </c>
       <c r="D87" s="12" t="s">
+        <v>300</v>
+      </c>
+      <c r="E87" s="19" t="s">
         <v>301</v>
-      </c>
-      <c r="E87" s="19" t="s">
-        <v>302</v>
       </c>
     </row>
     <row r="88" spans="1:5" s="6" customFormat="1" ht="38.25">
@@ -3228,7 +3232,7 @@
         <v>12</v>
       </c>
       <c r="D92" s="11" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="E92" s="16" t="s">
         <v>261</v>
@@ -3449,17 +3453,17 @@
       <c r="E104" s="22"/>
     </row>
     <row r="105" spans="1:5" ht="23.25">
-      <c r="A105" s="4">
+      <c r="A105" s="3">
         <f t="shared" si="1"/>
         <v>102</v>
       </c>
-      <c r="B105" s="15" t="s">
+      <c r="B105" s="14" t="s">
         <v>126</v>
       </c>
-      <c r="C105" s="15" t="s">
+      <c r="C105" s="14" t="s">
         <v>118</v>
       </c>
-      <c r="D105" s="15" t="s">
+      <c r="D105" s="14" t="s">
         <v>119</v>
       </c>
       <c r="E105" s="22"/>
@@ -3481,17 +3485,17 @@
       <c r="E106" s="22"/>
     </row>
     <row r="107" spans="1:5" ht="23.25">
-      <c r="A107" s="4">
+      <c r="A107" s="3">
         <f t="shared" si="1"/>
         <v>104</v>
       </c>
-      <c r="B107" s="15" t="s">
+      <c r="B107" s="14" t="s">
         <v>128</v>
       </c>
-      <c r="C107" s="15" t="s">
+      <c r="C107" s="14" t="s">
         <v>118</v>
       </c>
-      <c r="D107" s="15" t="s">
+      <c r="D107" s="14" t="s">
         <v>119</v>
       </c>
       <c r="E107" s="22"/>
@@ -3515,20 +3519,20 @@
       </c>
     </row>
     <row r="109" spans="1:5" ht="23.25">
-      <c r="A109" s="4">
+      <c r="A109" s="3">
         <f t="shared" si="1"/>
         <v>106</v>
       </c>
-      <c r="B109" s="15" t="s">
+      <c r="B109" s="14" t="s">
         <v>131</v>
       </c>
-      <c r="C109" s="15" t="s">
+      <c r="C109" s="14" t="s">
         <v>118</v>
       </c>
-      <c r="D109" s="15" t="s">
+      <c r="D109" s="14" t="s">
         <v>119</v>
       </c>
-      <c r="E109" s="21" t="s">
+      <c r="E109" s="20" t="s">
         <v>261</v>
       </c>
     </row>
@@ -3551,20 +3555,20 @@
       </c>
     </row>
     <row r="111" spans="1:5" s="5" customFormat="1" ht="25.5">
-      <c r="A111" s="4">
+      <c r="A111" s="3">
         <f t="shared" si="1"/>
         <v>108</v>
       </c>
-      <c r="B111" s="15" t="s">
+      <c r="B111" s="14" t="s">
         <v>293</v>
       </c>
-      <c r="C111" s="15" t="s">
+      <c r="C111" s="14" t="s">
         <v>134</v>
       </c>
-      <c r="D111" s="15" t="s">
+      <c r="D111" s="14" t="s">
         <v>133</v>
       </c>
-      <c r="E111" s="21" t="s">
+      <c r="E111" s="20" t="s">
         <v>261</v>
       </c>
     </row>

</xml_diff>

<commit_message>
+ screeningprograme email function * test case is completed
</commit_message>
<xml_diff>
--- a/docs/2010-10-11_Final Project Folder/TestCase1_30.xlsx
+++ b/docs/2010-10-11_Final Project Folder/TestCase1_30.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="440" uniqueCount="306">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="442" uniqueCount="308">
   <si>
     <t>CSSE3004/CSSE7024 Test Case</t>
     <phoneticPr fontId="0" type="noConversion"/>
@@ -982,6 +982,14 @@
   </si>
   <si>
     <t>F: need to implement the deletion function</t>
+  </si>
+  <si>
+    <t>P</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>P (email function sometimes failed due to the smtp server is unstable)</t>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -992,7 +1000,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -1030,13 +1038,13 @@
     </font>
     <font>
       <sz val="9"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="3"/>
       <charset val="136"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1058,12 +1066,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-4.9989318521683403E-2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1132,7 +1134,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1200,10 +1202,6 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="15" fontId="4" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
       <protection locked="0"/>
     </xf>
@@ -1503,11 +1501,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I112"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A94" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F74" sqref="F74"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="8" customWidth="1"/>
     <col min="2" max="2" width="31.140625" customWidth="1"/>
@@ -1558,7 +1556,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="38.25">
+    <row r="5" spans="1:9" ht="25.5">
       <c r="A5" s="4">
         <f>A4+1</f>
         <v>2</v>
@@ -1696,7 +1694,7 @@
       <c r="H11"/>
       <c r="I11"/>
     </row>
-    <row r="12" spans="1:9" ht="38.25">
+    <row r="12" spans="1:9" ht="25.5">
       <c r="A12" s="4">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -2194,7 +2192,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="37" spans="1:9" s="5" customFormat="1" ht="51">
+    <row r="37" spans="1:9" s="5" customFormat="1" ht="38.25">
       <c r="A37" s="4">
         <f t="shared" si="0"/>
         <v>34</v>
@@ -2314,7 +2312,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="43" spans="1:9" s="5" customFormat="1" ht="38.25">
+    <row r="43" spans="1:9" s="5" customFormat="1" ht="25.5">
       <c r="A43" s="4">
         <f t="shared" si="0"/>
         <v>40</v>
@@ -2336,7 +2334,7 @@
       <c r="H43"/>
       <c r="I43"/>
     </row>
-    <row r="44" spans="1:9" ht="51">
+    <row r="44" spans="1:9" ht="38.25">
       <c r="A44" s="4">
         <f t="shared" si="0"/>
         <v>41</v>
@@ -2398,7 +2396,7 @@
       <c r="H46"/>
       <c r="I46"/>
     </row>
-    <row r="47" spans="1:9" s="5" customFormat="1" ht="38.25">
+    <row r="47" spans="1:9" s="5" customFormat="1" ht="25.5">
       <c r="A47" s="4">
         <f t="shared" si="0"/>
         <v>44</v>
@@ -2745,7 +2743,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="64" spans="1:9" ht="38.25">
+    <row r="64" spans="1:9" ht="25.5">
       <c r="A64" s="4">
         <f t="shared" si="0"/>
         <v>61</v>
@@ -2903,9 +2901,11 @@
       <c r="D72" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="E72" s="22"/>
-    </row>
-    <row r="73" spans="1:5" s="5" customFormat="1" ht="25.5">
+      <c r="E72" s="18" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" s="5" customFormat="1" ht="38.25">
       <c r="A73" s="4">
         <f t="shared" si="1"/>
         <v>70</v>
@@ -2919,7 +2919,9 @@
       <c r="D73" s="13" t="s">
         <v>58</v>
       </c>
-      <c r="E73" s="22"/>
+      <c r="E73" s="17" t="s">
+        <v>307</v>
+      </c>
     </row>
     <row r="74" spans="1:5" ht="63.75">
       <c r="A74" s="4">
@@ -3101,7 +3103,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="84" spans="1:5" s="6" customFormat="1" ht="63.75">
+    <row r="84" spans="1:5" s="6" customFormat="1" ht="51">
       <c r="A84" s="4">
         <f t="shared" si="1"/>
         <v>81</v>
@@ -3209,7 +3211,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="90" spans="1:5" s="6" customFormat="1" ht="76.5">
+    <row r="90" spans="1:5" s="6" customFormat="1" ht="63.75">
       <c r="A90" s="4">
         <f t="shared" si="1"/>
         <v>87</v>
@@ -3353,7 +3355,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="98" spans="1:5" s="5" customFormat="1" ht="38.25">
+    <row r="98" spans="1:5" s="5" customFormat="1" ht="25.5">
       <c r="A98" s="4">
         <f t="shared" si="1"/>
         <v>95</v>
@@ -3371,7 +3373,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="99" spans="1:5" ht="38.25">
+    <row r="99" spans="1:5" ht="25.5">
       <c r="A99" s="4">
         <f t="shared" si="1"/>
         <v>96</v>
@@ -3461,7 +3463,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="104" spans="1:5" s="5" customFormat="1" ht="38.25">
+    <row r="104" spans="1:5" s="5" customFormat="1" ht="25.5">
       <c r="A104" s="4">
         <f t="shared" si="1"/>
         <v>101</v>
@@ -3636,7 +3638,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <sheetData/>
   <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3649,7 +3651,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <sheetData/>
   <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Update test cases 44 and 79
</commit_message>
<xml_diff>
--- a/docs/2010-10-11_Final Project Folder/TestCase1_30.xlsx
+++ b/docs/2010-10-11_Final Project Folder/TestCase1_30.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="-15" yWindow="-15" windowWidth="12045" windowHeight="5730"/>
@@ -14,7 +14,7 @@
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$E$112</definedName>
   </definedNames>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
@@ -946,10 +946,6 @@
     <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
-    <t>F: need to validate file format</t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
     <t xml:space="preserve">Confirm action - if confirmed, generate a random password and set this random password to the account.  </t>
     <phoneticPr fontId="6" type="noConversion"/>
   </si>
@@ -990,17 +986,20 @@
   <si>
     <t>P (email function sometimes failed due to the smtp server is unstable)</t>
     <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>P (cannot be done by design)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -1038,7 +1037,7 @@
     </font>
     <font>
       <sz val="9"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="136"/>
       <scheme val="minor"/>
@@ -1211,6 +1210,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -1289,6 +1293,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -1323,6 +1328,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1498,14 +1504,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I112"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F74" sqref="F74"/>
+    <sheetView tabSelected="1" topLeftCell="A40" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E47" sqref="E47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="8" customWidth="1"/>
     <col min="2" max="2" width="31.140625" customWidth="1"/>
@@ -1556,7 +1562,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="25.5">
+    <row r="5" spans="1:9" ht="38.25">
       <c r="A5" s="4">
         <f>A4+1</f>
         <v>2</v>
@@ -1694,7 +1700,7 @@
       <c r="H11"/>
       <c r="I11"/>
     </row>
-    <row r="12" spans="1:9" ht="25.5">
+    <row r="12" spans="1:9" ht="38.25">
       <c r="A12" s="4">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -1789,7 +1795,7 @@
         <v>171</v>
       </c>
       <c r="E16" s="18" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="17" spans="1:9" s="5" customFormat="1" ht="38.25">
@@ -1807,7 +1813,7 @@
         <v>171</v>
       </c>
       <c r="E17" s="17" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="F17"/>
       <c r="G17"/>
@@ -2192,7 +2198,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="37" spans="1:9" s="5" customFormat="1" ht="38.25">
+    <row r="37" spans="1:9" s="5" customFormat="1" ht="51">
       <c r="A37" s="4">
         <f t="shared" si="0"/>
         <v>34</v>
@@ -2312,7 +2318,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="43" spans="1:9" s="5" customFormat="1" ht="25.5">
+    <row r="43" spans="1:9" s="5" customFormat="1" ht="38.25">
       <c r="A43" s="4">
         <f t="shared" si="0"/>
         <v>40</v>
@@ -2334,7 +2340,7 @@
       <c r="H43"/>
       <c r="I43"/>
     </row>
-    <row r="44" spans="1:9" ht="38.25">
+    <row r="44" spans="1:9" ht="51">
       <c r="A44" s="4">
         <f t="shared" si="0"/>
         <v>41</v>
@@ -2396,7 +2402,7 @@
       <c r="H46"/>
       <c r="I46"/>
     </row>
-    <row r="47" spans="1:9" s="5" customFormat="1" ht="25.5">
+    <row r="47" spans="1:9" s="5" customFormat="1" ht="38.25">
       <c r="A47" s="4">
         <f t="shared" si="0"/>
         <v>44</v>
@@ -2411,7 +2417,7 @@
         <v>239</v>
       </c>
       <c r="E47" s="19" t="s">
-        <v>296</v>
+        <v>303</v>
       </c>
       <c r="F47"/>
       <c r="G47"/>
@@ -2667,7 +2673,7 @@
         <v>284</v>
       </c>
       <c r="E59" s="19" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="60" spans="1:9" ht="38.25">
@@ -2703,7 +2709,7 @@
         <v>92</v>
       </c>
       <c r="E61" s="17" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="62" spans="1:9" ht="63.75">
@@ -2721,7 +2727,7 @@
         <v>89</v>
       </c>
       <c r="E62" s="18" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="F62" s="5"/>
     </row>
@@ -2740,10 +2746,10 @@
         <v>86</v>
       </c>
       <c r="E63" s="17" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="64" spans="1:9" ht="25.5">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" ht="38.25">
       <c r="A64" s="4">
         <f t="shared" si="0"/>
         <v>61</v>
@@ -2758,7 +2764,7 @@
         <v>83</v>
       </c>
       <c r="E64" s="18" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="65" spans="1:5" s="5" customFormat="1" ht="63.75">
@@ -2776,7 +2782,7 @@
         <v>80</v>
       </c>
       <c r="E65" s="17" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="66" spans="1:5" ht="89.25">
@@ -2812,7 +2818,7 @@
         <v>74</v>
       </c>
       <c r="E67" s="17" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="68" spans="1:5" ht="25.5">
@@ -2830,7 +2836,7 @@
         <v>71</v>
       </c>
       <c r="E68" s="18" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="69" spans="1:5" s="5" customFormat="1" ht="25.5">
@@ -2848,7 +2854,7 @@
         <v>68</v>
       </c>
       <c r="E69" s="17" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="70" spans="1:5" ht="25.5">
@@ -2866,7 +2872,7 @@
         <v>50</v>
       </c>
       <c r="E70" s="18" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="71" spans="1:5" s="5" customFormat="1" ht="38.25">
@@ -2884,7 +2890,7 @@
         <v>30</v>
       </c>
       <c r="E71" s="17" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="72" spans="1:5" ht="25.5">
@@ -2902,7 +2908,7 @@
         <v>61</v>
       </c>
       <c r="E72" s="18" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="73" spans="1:5" s="5" customFormat="1" ht="38.25">
@@ -2920,7 +2926,7 @@
         <v>58</v>
       </c>
       <c r="E73" s="17" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="74" spans="1:5" ht="63.75">
@@ -3082,7 +3088,7 @@
         <v>33</v>
       </c>
       <c r="E82" s="18" t="s">
-        <v>294</v>
+        <v>307</v>
       </c>
     </row>
     <row r="83" spans="1:5" s="5" customFormat="1" ht="38.25">
@@ -3103,7 +3109,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="84" spans="1:5" s="6" customFormat="1" ht="51">
+    <row r="84" spans="1:5" s="6" customFormat="1" ht="63.75">
       <c r="A84" s="4">
         <f t="shared" si="1"/>
         <v>81</v>
@@ -3127,10 +3133,10 @@
         <v>82</v>
       </c>
       <c r="B85" s="12" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C85" s="12" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="D85" s="12" t="s">
         <v>9</v>
@@ -3169,10 +3175,10 @@
         <v>18</v>
       </c>
       <c r="D87" s="12" t="s">
+        <v>299</v>
+      </c>
+      <c r="E87" s="19" t="s">
         <v>300</v>
-      </c>
-      <c r="E87" s="19" t="s">
-        <v>301</v>
       </c>
     </row>
     <row r="88" spans="1:5" s="6" customFormat="1" ht="38.25">
@@ -3211,7 +3217,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="90" spans="1:5" s="6" customFormat="1" ht="63.75">
+    <row r="90" spans="1:5" s="6" customFormat="1" ht="76.5">
       <c r="A90" s="4">
         <f t="shared" si="1"/>
         <v>87</v>
@@ -3259,7 +3265,7 @@
         <v>12</v>
       </c>
       <c r="D92" s="11" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="E92" s="16" t="s">
         <v>261</v>
@@ -3355,7 +3361,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="98" spans="1:5" s="5" customFormat="1" ht="25.5">
+    <row r="98" spans="1:5" s="5" customFormat="1" ht="38.25">
       <c r="A98" s="4">
         <f t="shared" si="1"/>
         <v>95</v>
@@ -3373,7 +3379,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="99" spans="1:5" ht="25.5">
+    <row r="99" spans="1:5" ht="38.25">
       <c r="A99" s="4">
         <f t="shared" si="1"/>
         <v>96</v>
@@ -3463,7 +3469,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="104" spans="1:5" s="5" customFormat="1" ht="25.5">
+    <row r="104" spans="1:5" s="5" customFormat="1" ht="38.25">
       <c r="A104" s="4">
         <f t="shared" si="1"/>
         <v>101</v>
@@ -3478,7 +3484,7 @@
         <v>125</v>
       </c>
       <c r="E104" s="20" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="105" spans="1:5" ht="23.25">
@@ -3496,7 +3502,7 @@
         <v>119</v>
       </c>
       <c r="E105" s="21" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="106" spans="1:5" s="5" customFormat="1" ht="38.25">
@@ -3514,7 +3520,7 @@
         <v>122</v>
       </c>
       <c r="E106" s="20" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="107" spans="1:5" ht="23.25">
@@ -3532,7 +3538,7 @@
         <v>119</v>
       </c>
       <c r="E107" s="21" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="108" spans="1:5" s="5" customFormat="1" ht="38.25">
@@ -3622,7 +3628,7 @@
         <v>137</v>
       </c>
       <c r="E112" s="20" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
   </sheetData>
@@ -3633,12 +3639,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3646,12 +3652,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>